<commit_message>
terminado a rede neural para renatinha, funcionando!
</commit_message>
<xml_diff>
--- a/renatinha/escor.xlsx
+++ b/renatinha/escor.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19095" windowHeight="7815"/>
+    <workbookView windowWidth="14295" windowHeight="8835"/>
   </bookViews>
   <sheets>
     <sheet name="ESCOR" sheetId="1" r:id="rId1"/>
     <sheet name="IRIS" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ESCOR!$A$1:$F$116</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">ESCOR!$A$1:$E$116</definedName>
     <definedName name="_xlchart.v1.0" hidden="1">ESCOR!$B$1:$B$58</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">ESCOR!$B$59:$B$116</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">ESCOR!$B$1:$B$58</definedName>
@@ -56,11 +56,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="0.00000000000"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="0.00000000000"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="19">
     <font>
@@ -79,11 +79,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -95,46 +95,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -164,27 +126,26 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Cambria"/>
       <charset val="134"/>
       <scheme val="major"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -202,7 +163,46 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -229,19 +229,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -259,13 +265,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -277,13 +307,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -295,25 +355,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -325,31 +385,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -361,49 +397,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,15 +432,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -460,16 +451,18 @@
       <right/>
       <top/>
       <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.399975585192419"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -506,11 +499,27 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.399975585192419"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -529,78 +538,69 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -961,22 +961,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F116"/>
+  <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="14.6666666666667" style="3" customWidth="1"/>
     <col min="2" max="2" width="15.6666666666667" style="3" customWidth="1"/>
     <col min="3" max="3" width="15.44" style="3" customWidth="1"/>
-    <col min="4" max="5" width="14.5533333333333" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
+    <col min="4" max="4" width="14.5533333333333" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5">
       <c r="A1" s="3">
         <v>11.0339</v>
       </c>
@@ -992,11 +992,8 @@
       <c r="E1">
         <v>1</v>
       </c>
-      <c r="F1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" s="3">
         <v>10.9587</v>
       </c>
@@ -1012,11 +1009,8 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="3">
         <v>8.67351</v>
       </c>
@@ -1032,11 +1026,8 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="3">
         <v>2.36073</v>
       </c>
@@ -1052,11 +1043,8 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="3">
         <v>10.7938</v>
       </c>
@@ -1072,11 +1060,8 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="3">
         <v>10.9292</v>
       </c>
@@ -1092,11 +1077,8 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" s="3">
         <v>17.8989</v>
       </c>
@@ -1112,11 +1094,8 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" s="3">
         <v>5.18293</v>
       </c>
@@ -1132,11 +1111,8 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" s="3">
         <v>1.90875</v>
       </c>
@@ -1152,11 +1128,8 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" s="3">
         <v>21.1604</v>
       </c>
@@ -1172,11 +1145,8 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" s="3">
         <v>4.31251</v>
       </c>
@@ -1192,11 +1162,8 @@
       <c r="E11">
         <v>1</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" s="3">
         <v>4.86351</v>
       </c>
@@ -1212,11 +1179,8 @@
       <c r="E12">
         <v>1</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="3">
         <v>3.82778</v>
       </c>
@@ -1232,11 +1196,8 @@
       <c r="E13">
         <v>1</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" s="3">
         <v>0.620509</v>
       </c>
@@ -1252,11 +1213,8 @@
       <c r="E14">
         <v>1</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="3">
         <v>8.51851</v>
       </c>
@@ -1272,11 +1230,8 @@
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="3">
         <v>11.0773</v>
       </c>
@@ -1292,11 +1247,8 @@
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="3">
         <v>13.5762</v>
       </c>
@@ -1312,11 +1264,8 @@
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="3">
         <v>3.33878</v>
       </c>
@@ -1332,11 +1281,8 @@
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="3">
         <v>0.786286</v>
       </c>
@@ -1352,11 +1298,8 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="3">
         <v>16.0245</v>
       </c>
@@ -1372,11 +1315,8 @@
       <c r="E20">
         <v>1</v>
       </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="3">
         <v>2.4397</v>
       </c>
@@ -1392,11 +1332,8 @@
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="3">
         <v>2.71544</v>
       </c>
@@ -1412,11 +1349,8 @@
       <c r="E22">
         <v>1</v>
       </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="3">
         <v>3.79582</v>
       </c>
@@ -1432,11 +1366,8 @@
       <c r="E23">
         <v>1</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="3">
         <v>1.6098</v>
       </c>
@@ -1452,11 +1383,8 @@
       <c r="E24">
         <v>1</v>
       </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="3">
         <v>9.85452</v>
       </c>
@@ -1472,11 +1400,8 @@
       <c r="E25">
         <v>1</v>
       </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="3">
         <v>18.3397</v>
       </c>
@@ -1492,11 +1417,8 @@
       <c r="E26">
         <v>1</v>
       </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="3">
         <v>14.6727</v>
       </c>
@@ -1512,11 +1434,8 @@
       <c r="E27">
         <v>1</v>
       </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="3">
         <v>11.0551</v>
       </c>
@@ -1532,11 +1451,8 @@
       <c r="E28">
         <v>1</v>
       </c>
-      <c r="F28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="3">
         <v>3.06664</v>
       </c>
@@ -1552,11 +1468,8 @@
       <c r="E29">
         <v>1</v>
       </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="3">
         <v>4.18596</v>
       </c>
@@ -1572,11 +1485,8 @@
       <c r="E30">
         <v>1</v>
       </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="3">
         <v>11.2812</v>
       </c>
@@ -1592,11 +1502,8 @@
       <c r="E31">
         <v>1</v>
       </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="3">
         <v>1.8486</v>
       </c>
@@ -1612,11 +1519,8 @@
       <c r="E32">
         <v>1</v>
       </c>
-      <c r="F32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="3">
         <v>11.1327</v>
       </c>
@@ -1632,11 +1536,8 @@
       <c r="E33">
         <v>1</v>
       </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="3">
         <v>19.1598</v>
       </c>
@@ -1652,11 +1553,8 @@
       <c r="E34">
         <v>1</v>
       </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="3">
         <v>13.0662</v>
       </c>
@@ -1672,11 +1570,8 @@
       <c r="E35">
         <v>1</v>
       </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="3">
         <v>13.1726</v>
       </c>
@@ -1692,11 +1587,8 @@
       <c r="E36">
         <v>1</v>
       </c>
-      <c r="F36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="3">
         <v>0.272141</v>
       </c>
@@ -1712,11 +1604,8 @@
       <c r="E37">
         <v>1</v>
       </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="3">
         <v>20.9118</v>
       </c>
@@ -1732,11 +1621,8 @@
       <c r="E38">
         <v>1</v>
       </c>
-      <c r="F38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="3">
         <v>17.2504</v>
       </c>
@@ -1752,11 +1638,8 @@
       <c r="E39">
         <v>1</v>
       </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="3">
         <v>6.6035</v>
       </c>
@@ -1772,11 +1655,8 @@
       <c r="E40">
         <v>1</v>
       </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="3">
         <v>9.25387</v>
       </c>
@@ -1792,11 +1672,8 @@
       <c r="E41">
         <v>1</v>
       </c>
-      <c r="F41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="3">
         <v>5.05648</v>
       </c>
@@ -1812,11 +1689,8 @@
       <c r="E42">
         <v>1</v>
       </c>
-      <c r="F42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="3">
         <v>23.8562</v>
       </c>
@@ -1832,11 +1706,8 @@
       <c r="E43">
         <v>1</v>
       </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="3">
         <v>17.5409</v>
       </c>
@@ -1852,11 +1723,8 @@
       <c r="E44">
         <v>1</v>
       </c>
-      <c r="F44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="3">
         <v>16.2659</v>
       </c>
@@ -1872,11 +1740,8 @@
       <c r="E45">
         <v>1</v>
       </c>
-      <c r="F45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="3">
         <v>11.1917</v>
       </c>
@@ -1892,11 +1757,8 @@
       <c r="E46">
         <v>1</v>
       </c>
-      <c r="F46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="3">
         <v>3.00538</v>
       </c>
@@ -1912,11 +1774,8 @@
       <c r="E47">
         <v>1</v>
       </c>
-      <c r="F47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="3">
         <v>2.46455</v>
       </c>
@@ -1932,11 +1791,8 @@
       <c r="E48">
         <v>1</v>
       </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="3">
         <v>7.12846</v>
       </c>
@@ -1952,11 +1808,8 @@
       <c r="E49">
         <v>1</v>
       </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="3">
         <v>0.414764</v>
       </c>
@@ -1972,11 +1825,8 @@
       <c r="E50">
         <v>1</v>
       </c>
-      <c r="F50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6">
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="3">
         <v>5.14811</v>
       </c>
@@ -1992,11 +1842,8 @@
       <c r="E51">
         <v>1</v>
       </c>
-      <c r="F51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6">
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="3">
         <v>22.7154</v>
       </c>
@@ -2012,11 +1859,8 @@
       <c r="E52">
         <v>1</v>
       </c>
-      <c r="F52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6">
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="3">
         <v>9.38378</v>
       </c>
@@ -2032,11 +1876,8 @@
       <c r="E53">
         <v>1</v>
       </c>
-      <c r="F53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6">
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" s="3">
         <v>7.16352</v>
       </c>
@@ -2052,11 +1893,8 @@
       <c r="E54">
         <v>1</v>
       </c>
-      <c r="F54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6">
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" s="3">
         <v>5.5228</v>
       </c>
@@ -2072,11 +1910,8 @@
       <c r="E55">
         <v>1</v>
       </c>
-      <c r="F55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6">
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" s="3">
         <v>16.8717</v>
       </c>
@@ -2092,11 +1927,8 @@
       <c r="E56">
         <v>1</v>
       </c>
-      <c r="F56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6">
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" s="3">
         <v>18.2273</v>
       </c>
@@ -2112,11 +1944,8 @@
       <c r="E57">
         <v>1</v>
       </c>
-      <c r="F57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" s="3">
         <v>18.302</v>
       </c>
@@ -2132,11 +1961,8 @@
       <c r="E58">
         <v>1</v>
       </c>
-      <c r="F58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6">
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" s="3">
         <v>38.5887</v>
       </c>
@@ -2150,13 +1976,10 @@
         <v>7.47987</v>
       </c>
       <c r="E59">
-        <v>1</v>
-      </c>
-      <c r="F59">
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:5">
       <c r="A60" s="3">
         <v>33.7719</v>
       </c>
@@ -2170,13 +1993,10 @@
         <v>1.09552</v>
       </c>
       <c r="E60">
-        <v>1</v>
-      </c>
-      <c r="F60">
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:5">
       <c r="A61" s="3">
         <v>37.1545</v>
       </c>
@@ -2190,13 +2010,10 @@
         <v>2.06911</v>
       </c>
       <c r="E61">
-        <v>1</v>
-      </c>
-      <c r="F61">
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:5">
       <c r="A62" s="3">
         <v>25.6261</v>
       </c>
@@ -2210,13 +2027,10 @@
         <v>5.53866</v>
       </c>
       <c r="E62">
-        <v>1</v>
-      </c>
-      <c r="F62">
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:5">
       <c r="A63" s="3">
         <v>47.8786</v>
       </c>
@@ -2230,13 +2044,10 @@
         <v>1.28564</v>
       </c>
       <c r="E63">
-        <v>1</v>
-      </c>
-      <c r="F63">
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:5">
       <c r="A64" s="3">
         <v>50.4886</v>
       </c>
@@ -2250,13 +2061,10 @@
         <v>0.500376</v>
       </c>
       <c r="E64">
-        <v>1</v>
-      </c>
-      <c r="F64">
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:5">
       <c r="A65" s="3">
         <v>28.9972</v>
       </c>
@@ -2270,13 +2078,10 @@
         <v>3.7682</v>
       </c>
       <c r="E65">
-        <v>1</v>
-      </c>
-      <c r="F65">
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:5">
       <c r="A66" s="3">
         <v>31.2199</v>
       </c>
@@ -2290,13 +2095,10 @@
         <v>4.37192</v>
       </c>
       <c r="E66">
-        <v>1</v>
-      </c>
-      <c r="F66">
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:5">
       <c r="A67" s="3">
         <v>21.3844</v>
       </c>
@@ -2310,13 +2112,10 @@
         <v>3.82793</v>
       </c>
       <c r="E67">
-        <v>1</v>
-      </c>
-      <c r="F67">
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:5">
       <c r="A68" s="3">
         <v>36.8935</v>
       </c>
@@ -2330,13 +2129,10 @@
         <v>4.11547</v>
       </c>
       <c r="E68">
-        <v>1</v>
-      </c>
-      <c r="F68">
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:5">
       <c r="A69" s="3">
         <v>29.6673</v>
       </c>
@@ -2350,13 +2146,10 @@
         <v>2.35452</v>
       </c>
       <c r="E69">
-        <v>1</v>
-      </c>
-      <c r="F69">
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:5">
       <c r="A70" s="3">
         <v>42.2754</v>
       </c>
@@ -2370,13 +2163,10 @@
         <v>3.62161</v>
       </c>
       <c r="E70">
-        <v>1</v>
-      </c>
-      <c r="F70">
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:5">
       <c r="A71" s="3">
         <v>40.5242</v>
       </c>
@@ -2390,13 +2180,10 @@
         <v>4.63421</v>
       </c>
       <c r="E71">
-        <v>1</v>
-      </c>
-      <c r="F71">
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:5">
       <c r="A72" s="3">
         <v>49.2582</v>
       </c>
@@ -2410,13 +2197,10 @@
         <v>3.18302</v>
       </c>
       <c r="E72">
-        <v>1</v>
-      </c>
-      <c r="F72">
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:5">
       <c r="A73" s="3">
         <v>33.1439</v>
       </c>
@@ -2430,13 +2214,10 @@
         <v>2.50564</v>
       </c>
       <c r="E73">
-        <v>1</v>
-      </c>
-      <c r="F73">
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:5">
       <c r="A74" s="3">
         <v>41.4024</v>
       </c>
@@ -2450,13 +2231,10 @@
         <v>4.07715</v>
       </c>
       <c r="E74">
-        <v>1</v>
-      </c>
-      <c r="F74">
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:5">
       <c r="A75" s="3">
         <v>48.9977</v>
       </c>
@@ -2470,13 +2248,10 @@
         <v>0.553145</v>
       </c>
       <c r="E75">
-        <v>1</v>
-      </c>
-      <c r="F75">
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:5">
       <c r="A76" s="3">
         <v>36.5936</v>
       </c>
@@ -2490,13 +2265,10 @@
         <v>2.60033</v>
       </c>
       <c r="E76">
-        <v>1</v>
-      </c>
-      <c r="F76">
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:5">
       <c r="A77" s="3">
         <v>32.5251</v>
       </c>
@@ -2510,13 +2282,10 @@
         <v>6.21823</v>
       </c>
       <c r="E77">
-        <v>1</v>
-      </c>
-      <c r="F77">
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:5">
       <c r="A78" s="3">
         <v>43.8601</v>
       </c>
@@ -2530,13 +2299,10 @@
         <v>0.732949</v>
       </c>
       <c r="E78">
-        <v>1</v>
-      </c>
-      <c r="F78">
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:5">
       <c r="A79" s="3">
         <v>38.8123</v>
       </c>
@@ -2550,13 +2316,10 @@
         <v>1.60399</v>
       </c>
       <c r="E79">
-        <v>1</v>
-      </c>
-      <c r="F79">
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:5">
       <c r="A80" s="3">
         <v>31.3518</v>
       </c>
@@ -2570,13 +2333,10 @@
         <v>4.2332</v>
       </c>
       <c r="E80">
-        <v>1</v>
-      </c>
-      <c r="F80">
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:5">
       <c r="A81" s="3">
         <v>43.9203</v>
       </c>
@@ -2590,13 +2350,10 @@
         <v>1.42399</v>
       </c>
       <c r="E81">
-        <v>1</v>
-      </c>
-      <c r="F81">
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:5">
       <c r="A82" s="3">
         <v>52.7818</v>
       </c>
@@ -2610,13 +2367,10 @@
         <v>2.20987</v>
       </c>
       <c r="E82">
-        <v>1</v>
-      </c>
-      <c r="F82">
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:5">
       <c r="A83" s="3">
         <v>33.4843</v>
       </c>
@@ -2630,13 +2384,10 @@
         <v>2.20502</v>
       </c>
       <c r="E83">
-        <v>1</v>
-      </c>
-      <c r="F83">
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:5">
       <c r="A84" s="3">
         <v>38.7062</v>
       </c>
@@ -2650,13 +2401,10 @@
         <v>1.60778</v>
       </c>
       <c r="E84">
-        <v>1</v>
-      </c>
-      <c r="F84">
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:5">
       <c r="A85" s="3">
         <v>42.9567</v>
       </c>
@@ -2670,13 +2418,10 @@
         <v>4.09674</v>
       </c>
       <c r="E85">
-        <v>1</v>
-      </c>
-      <c r="F85">
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:5">
       <c r="A86" s="3">
         <v>38.4165</v>
       </c>
@@ -2690,13 +2435,10 @@
         <v>0.925003</v>
       </c>
       <c r="E86">
-        <v>1</v>
-      </c>
-      <c r="F86">
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:5">
       <c r="A87" s="3">
         <v>45.4333</v>
       </c>
@@ -2710,13 +2452,10 @@
         <v>4.50666</v>
       </c>
       <c r="E87">
-        <v>1</v>
-      </c>
-      <c r="F87">
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:5">
       <c r="A88" s="3">
         <v>48.3039</v>
       </c>
@@ -2730,13 +2469,10 @@
         <v>3.28561</v>
       </c>
       <c r="E88">
-        <v>1</v>
-      </c>
-      <c r="F88">
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:5">
       <c r="A89" s="3">
         <v>42.7683</v>
       </c>
@@ -2750,13 +2486,10 @@
         <v>0.771127</v>
       </c>
       <c r="E89">
-        <v>1</v>
-      </c>
-      <c r="F89">
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:5">
       <c r="A90" s="3">
         <v>44.7357</v>
       </c>
@@ -2770,13 +2503,10 @@
         <v>3.47496</v>
       </c>
       <c r="E90">
-        <v>1</v>
-      </c>
-      <c r="F90">
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:5">
       <c r="A91" s="3">
         <v>46.6177</v>
       </c>
@@ -2790,13 +2520,10 @@
         <v>0.636649</v>
       </c>
       <c r="E91">
-        <v>1</v>
-      </c>
-      <c r="F91">
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:6">
+    <row r="92" spans="1:5">
       <c r="A92" s="3">
         <v>34.1074</v>
       </c>
@@ -2810,13 +2537,10 @@
         <v>3.02879</v>
       </c>
       <c r="E92">
-        <v>1</v>
-      </c>
-      <c r="F92">
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:5">
       <c r="A93" s="3">
         <v>34.0116</v>
       </c>
@@ -2830,13 +2554,10 @@
         <v>3.57139</v>
       </c>
       <c r="E93">
-        <v>1</v>
-      </c>
-      <c r="F93">
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:5">
       <c r="A94" s="3">
         <v>19.9626</v>
       </c>
@@ -2850,13 +2571,10 @@
         <v>1.70586</v>
       </c>
       <c r="E94">
-        <v>1</v>
-      </c>
-      <c r="F94">
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:5">
       <c r="A95" s="3">
         <v>34.4978</v>
       </c>
@@ -2870,13 +2588,10 @@
         <v>4.7318</v>
       </c>
       <c r="E95">
-        <v>1</v>
-      </c>
-      <c r="F95">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:5">
       <c r="A96" s="3">
         <v>42.4842</v>
       </c>
@@ -2890,13 +2605,10 @@
         <v>0.781078</v>
       </c>
       <c r="E96">
-        <v>1</v>
-      </c>
-      <c r="F96">
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:6">
+    <row r="97" spans="1:5">
       <c r="A97" s="3">
         <v>32.1446</v>
       </c>
@@ -2910,13 +2622,10 @@
         <v>3.55565</v>
       </c>
       <c r="E97">
-        <v>1</v>
-      </c>
-      <c r="F97">
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:6">
+    <row r="98" spans="1:5">
       <c r="A98" s="3">
         <v>57.0419</v>
       </c>
@@ -2930,13 +2639,10 @@
         <v>3.20429</v>
       </c>
       <c r="E98">
-        <v>1</v>
-      </c>
-      <c r="F98">
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:6">
+    <row r="99" spans="1:5">
       <c r="A99" s="3">
         <v>38.6755</v>
       </c>
@@ -2950,13 +2656,10 @@
         <v>2.70749</v>
       </c>
       <c r="E99">
-        <v>1</v>
-      </c>
-      <c r="F99">
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6">
+    <row r="100" spans="1:5">
       <c r="A100" s="3">
         <v>37.7916</v>
       </c>
@@ -2970,13 +2673,10 @@
         <v>3.34536</v>
       </c>
       <c r="E100">
-        <v>1</v>
-      </c>
-      <c r="F100">
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6">
+    <row r="101" spans="1:5">
       <c r="A101" s="3">
         <v>46.5002</v>
       </c>
@@ -2990,13 +2690,10 @@
         <v>1.3339</v>
       </c>
       <c r="E101">
-        <v>1</v>
-      </c>
-      <c r="F101">
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:6">
+    <row r="102" spans="1:5">
       <c r="A102" s="3">
         <v>20.5793</v>
       </c>
@@ -3010,13 +2707,10 @@
         <v>1.67274</v>
       </c>
       <c r="E102">
-        <v>1</v>
-      </c>
-      <c r="F102">
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6">
+    <row r="103" spans="1:5">
       <c r="A103" s="3">
         <v>28.9745</v>
       </c>
@@ -3030,13 +2724,10 @@
         <v>3.07599</v>
       </c>
       <c r="E103">
-        <v>1</v>
-      </c>
-      <c r="F103">
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6">
+    <row r="104" spans="1:5">
       <c r="A104" s="3">
         <v>58.5627</v>
       </c>
@@ -3050,13 +2741,10 @@
         <v>1.58727</v>
       </c>
       <c r="E104">
-        <v>1</v>
-      </c>
-      <c r="F104">
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6">
+    <row r="105" spans="1:5">
       <c r="A105" s="3">
         <v>38.1563</v>
       </c>
@@ -3070,13 +2758,10 @@
         <v>5.15385</v>
       </c>
       <c r="E105">
-        <v>1</v>
-      </c>
-      <c r="F105">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6">
+    <row r="106" spans="1:5">
       <c r="A106" s="3">
         <v>41.9338</v>
       </c>
@@ -3090,13 +2775,10 @@
         <v>4.67158</v>
       </c>
       <c r="E106">
-        <v>1</v>
-      </c>
-      <c r="F106">
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6">
+    <row r="107" spans="1:5">
       <c r="A107" s="3">
         <v>28.6015</v>
       </c>
@@ -3110,13 +2792,10 @@
         <v>8.91298</v>
       </c>
       <c r="E107">
-        <v>1</v>
-      </c>
-      <c r="F107">
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6">
+    <row r="108" spans="1:5">
       <c r="A108" s="3">
         <v>36.2327</v>
       </c>
@@ -3130,13 +2809,10 @@
         <v>4.55943</v>
       </c>
       <c r="E108">
-        <v>1</v>
-      </c>
-      <c r="F108">
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6">
+    <row r="109" spans="1:5">
       <c r="A109" s="3">
         <v>40.5814</v>
       </c>
@@ -3150,13 +2826,10 @@
         <v>3.89252</v>
       </c>
       <c r="E109">
-        <v>1</v>
-      </c>
-      <c r="F109">
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:6">
+    <row r="110" spans="1:5">
       <c r="A110" s="3">
         <v>43.7848</v>
       </c>
@@ -3170,13 +2843,10 @@
         <v>1.83419</v>
       </c>
       <c r="E110">
-        <v>1</v>
-      </c>
-      <c r="F110">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:6">
+    <row r="111" spans="1:5">
       <c r="A111" s="3">
         <v>34.8769</v>
       </c>
@@ -3190,13 +2860,10 @@
         <v>2.15272</v>
       </c>
       <c r="E111">
-        <v>1</v>
-      </c>
-      <c r="F111">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:6">
+    <row r="112" spans="1:5">
       <c r="A112" s="3">
         <v>38.7435</v>
       </c>
@@ -3210,13 +2877,10 @@
         <v>4.20914</v>
       </c>
       <c r="E112">
-        <v>1</v>
-      </c>
-      <c r="F112">
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:6">
+    <row r="113" spans="1:5">
       <c r="A113" s="3">
         <v>36.2735</v>
       </c>
@@ -3230,13 +2894,10 @@
         <v>2.61202</v>
       </c>
       <c r="E113">
-        <v>1</v>
-      </c>
-      <c r="F113">
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6">
+    <row r="114" spans="1:5">
       <c r="A114" s="3">
         <v>27.0122</v>
       </c>
@@ -3250,13 +2911,10 @@
         <v>3.56412</v>
       </c>
       <c r="E114">
-        <v>1</v>
-      </c>
-      <c r="F114">
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:6">
+    <row r="115" spans="1:5">
       <c r="A115" s="3">
         <v>24.2037</v>
       </c>
@@ -3270,13 +2928,10 @@
         <v>3.43869</v>
       </c>
       <c r="E115">
-        <v>1</v>
-      </c>
-      <c r="F115">
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6">
+    <row r="116" spans="1:5">
       <c r="A116" s="3">
         <v>7.59356</v>
       </c>
@@ -3290,9 +2945,6 @@
         <v>4.49995</v>
       </c>
       <c r="E116">
-        <v>1</v>
-      </c>
-      <c r="F116">
         <v>0</v>
       </c>
     </row>

</xml_diff>